<commit_message>
NASA_TLX now has frames
</commit_message>
<xml_diff>
--- a/src/app/study_files/downloads/NASA_TLX.xlsx
+++ b/src/app/study_files/downloads/NASA_TLX.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bosch-my.sharepoint.com/personal/iim6fe_bosch_com/Documents/PersonalDrive/BA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="13_ncr:1_{089E37D3-B48C-4311-9CC9-A6A49908B007}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{99EE9D51-7B6A-4EB0-ABB8-F947D99ADB1F}"/>
+  <xr:revisionPtr revIDLastSave="46" documentId="13_ncr:1_{089E37D3-B48C-4311-9CC9-A6A49908B007}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E83254E2-1C8D-47B9-99EB-6D67566CE7E4}"/>
   <bookViews>
-    <workbookView xWindow="-31725" yWindow="2730" windowWidth="28800" windowHeight="15345" xr2:uid="{28D2DBF4-2DB2-4CB6-9F9C-C7B60EF5AF83}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="28800" windowHeight="15345" xr2:uid="{28D2DBF4-2DB2-4CB6-9F9C-C7B60EF5AF83}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -341,7 +341,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -379,11 +379,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -393,9 +413,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -413,21 +430,38 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -747,8 +781,8 @@
   </sheetPr>
   <dimension ref="B1:AB68"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AC27" sqref="AC27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -767,354 +801,354 @@
   <sheetData>
     <row r="1" spans="2:28" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:28" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
-      <c r="N2" s="9"/>
-      <c r="O2" s="9"/>
-      <c r="P2" s="9"/>
-      <c r="Q2" s="9"/>
-      <c r="R2" s="9"/>
-      <c r="S2" s="9"/>
-      <c r="T2" s="9"/>
-      <c r="U2" s="9"/>
-      <c r="V2" s="9"/>
-      <c r="W2" s="9"/>
-      <c r="X2" s="9"/>
-      <c r="Y2" s="9"/>
-      <c r="Z2" s="9"/>
-      <c r="AA2" s="9"/>
-      <c r="AB2" s="9"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
+      <c r="P2" s="8"/>
+      <c r="Q2" s="8"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+      <c r="U2" s="8"/>
+      <c r="V2" s="8"/>
+      <c r="W2" s="8"/>
+      <c r="X2" s="8"/>
+      <c r="Y2" s="8"/>
+      <c r="Z2" s="8"/>
+      <c r="AA2" s="8"/>
+      <c r="AB2" s="8"/>
     </row>
     <row r="3" spans="2:28" ht="51.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="4" spans="2:28" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="14"/>
-      <c r="M4" s="14"/>
-      <c r="N4" s="14"/>
-      <c r="O4" s="14"/>
-      <c r="P4" s="14"/>
-      <c r="Q4" s="14"/>
-      <c r="R4" s="14"/>
-      <c r="S4" s="14"/>
-      <c r="T4" s="14"/>
-      <c r="U4" s="14"/>
-      <c r="V4" s="14"/>
-      <c r="W4" s="14"/>
-      <c r="X4" s="14"/>
-      <c r="Y4" s="14"/>
-      <c r="Z4" s="14"/>
-      <c r="AA4" s="14"/>
-      <c r="AB4" s="14"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="10"/>
+      <c r="R4" s="10"/>
+      <c r="S4" s="10"/>
+      <c r="T4" s="10"/>
+      <c r="U4" s="10"/>
+      <c r="V4" s="10"/>
+      <c r="W4" s="10"/>
+      <c r="X4" s="10"/>
+      <c r="Y4" s="10"/>
+      <c r="Z4" s="10"/>
+      <c r="AA4" s="10"/>
+      <c r="AB4" s="10"/>
     </row>
     <row r="5" spans="2:28" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="6"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="7"/>
-      <c r="O5" s="7"/>
-      <c r="P5" s="7"/>
-      <c r="Q5" s="7"/>
-      <c r="R5" s="7"/>
-      <c r="S5" s="7"/>
-      <c r="T5" s="7"/>
-      <c r="U5" s="7"/>
-      <c r="V5" s="7"/>
-      <c r="W5" s="7"/>
-      <c r="X5" s="7"/>
-      <c r="Y5" s="7"/>
-      <c r="Z5" s="7"/>
-      <c r="AA5" s="7"/>
-      <c r="AB5" s="7"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6"/>
+      <c r="S5" s="6"/>
+      <c r="T5" s="6"/>
+      <c r="U5" s="6"/>
+      <c r="V5" s="6"/>
+      <c r="W5" s="6"/>
+      <c r="X5" s="6"/>
+      <c r="Y5" s="6"/>
+      <c r="Z5" s="6"/>
+      <c r="AA5" s="6"/>
+      <c r="AB5" s="6"/>
     </row>
     <row r="6" spans="2:28" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15"/>
-      <c r="K6" s="15"/>
-      <c r="L6" s="15"/>
-      <c r="M6" s="15"/>
-      <c r="N6" s="15"/>
-      <c r="O6" s="15"/>
-      <c r="P6" s="15"/>
-      <c r="Q6" s="15"/>
-      <c r="R6" s="15"/>
-      <c r="S6" s="15"/>
-      <c r="T6" s="15"/>
-      <c r="U6" s="15"/>
-      <c r="V6" s="15"/>
-      <c r="W6" s="15"/>
-      <c r="X6" s="15"/>
-      <c r="Y6" s="15"/>
-      <c r="Z6" s="15"/>
-      <c r="AA6" s="15"/>
-      <c r="AB6" s="15"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="11"/>
+      <c r="P6" s="11"/>
+      <c r="Q6" s="11"/>
+      <c r="R6" s="11"/>
+      <c r="S6" s="11"/>
+      <c r="T6" s="11"/>
+      <c r="U6" s="11"/>
+      <c r="V6" s="11"/>
+      <c r="W6" s="11"/>
+      <c r="X6" s="11"/>
+      <c r="Y6" s="11"/>
+      <c r="Z6" s="11"/>
+      <c r="AA6" s="11"/>
+      <c r="AB6" s="11"/>
     </row>
     <row r="7" spans="2:28" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="6"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="8"/>
-      <c r="N7" s="8"/>
-      <c r="O7" s="8"/>
-      <c r="P7" s="8"/>
-      <c r="Q7" s="8"/>
-      <c r="R7" s="8"/>
-      <c r="S7" s="8"/>
-      <c r="T7" s="8"/>
-      <c r="U7" s="8"/>
-      <c r="V7" s="8"/>
-      <c r="W7" s="8"/>
-      <c r="X7" s="8"/>
-      <c r="Y7" s="8"/>
-      <c r="Z7" s="8"/>
-      <c r="AA7" s="8"/>
-      <c r="AB7" s="8"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="7"/>
+      <c r="O7" s="7"/>
+      <c r="P7" s="7"/>
+      <c r="Q7" s="7"/>
+      <c r="R7" s="7"/>
+      <c r="S7" s="7"/>
+      <c r="T7" s="7"/>
+      <c r="U7" s="7"/>
+      <c r="V7" s="7"/>
+      <c r="W7" s="7"/>
+      <c r="X7" s="7"/>
+      <c r="Y7" s="7"/>
+      <c r="Z7" s="7"/>
+      <c r="AA7" s="7"/>
+      <c r="AB7" s="7"/>
     </row>
     <row r="8" spans="2:28" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="15"/>
-      <c r="M8" s="15"/>
-      <c r="N8" s="15"/>
-      <c r="O8" s="15"/>
-      <c r="P8" s="15"/>
-      <c r="Q8" s="15"/>
-      <c r="R8" s="15"/>
-      <c r="S8" s="15"/>
-      <c r="T8" s="15"/>
-      <c r="U8" s="15"/>
-      <c r="V8" s="15"/>
-      <c r="W8" s="15"/>
-      <c r="X8" s="15"/>
-      <c r="Y8" s="15"/>
-      <c r="Z8" s="15"/>
-      <c r="AA8" s="15"/>
-      <c r="AB8" s="15"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="11"/>
+      <c r="O8" s="11"/>
+      <c r="P8" s="11"/>
+      <c r="Q8" s="11"/>
+      <c r="R8" s="11"/>
+      <c r="S8" s="11"/>
+      <c r="T8" s="11"/>
+      <c r="U8" s="11"/>
+      <c r="V8" s="11"/>
+      <c r="W8" s="11"/>
+      <c r="X8" s="11"/>
+      <c r="Y8" s="11"/>
+      <c r="Z8" s="11"/>
+      <c r="AA8" s="11"/>
+      <c r="AB8" s="11"/>
     </row>
     <row r="10" spans="2:28" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="13"/>
-      <c r="N10" s="13"/>
-      <c r="O10" s="13"/>
-      <c r="P10" s="13"/>
-      <c r="Q10" s="13"/>
-      <c r="R10" s="13"/>
-      <c r="S10" s="13"/>
-      <c r="T10" s="13"/>
-      <c r="U10" s="13"/>
-      <c r="V10" s="13"/>
-      <c r="W10" s="13"/>
-      <c r="X10" s="13"/>
-      <c r="Y10" s="13"/>
-      <c r="Z10" s="13"/>
-      <c r="AA10" s="13"/>
-      <c r="AB10" s="13"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="12"/>
+      <c r="N10" s="12"/>
+      <c r="O10" s="12"/>
+      <c r="P10" s="12"/>
+      <c r="Q10" s="12"/>
+      <c r="R10" s="12"/>
+      <c r="S10" s="12"/>
+      <c r="T10" s="12"/>
+      <c r="U10" s="12"/>
+      <c r="V10" s="12"/>
+      <c r="W10" s="12"/>
+      <c r="X10" s="12"/>
+      <c r="Y10" s="12"/>
+      <c r="Z10" s="12"/>
+      <c r="AA10" s="12"/>
+      <c r="AB10" s="12"/>
     </row>
     <row r="12" spans="2:28" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="13"/>
-      <c r="K12" s="13"/>
-      <c r="L12" s="13"/>
-      <c r="M12" s="13"/>
-      <c r="N12" s="13"/>
-      <c r="O12" s="13"/>
-      <c r="P12" s="13"/>
-      <c r="Q12" s="13"/>
-      <c r="R12" s="13"/>
-      <c r="S12" s="13"/>
-      <c r="T12" s="13"/>
-      <c r="U12" s="13"/>
-      <c r="V12" s="13"/>
-      <c r="W12" s="13"/>
-      <c r="X12" s="13"/>
-      <c r="Y12" s="13"/>
-      <c r="Z12" s="13"/>
-      <c r="AA12" s="13"/>
-      <c r="AB12" s="13"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="12"/>
+      <c r="M12" s="12"/>
+      <c r="N12" s="12"/>
+      <c r="O12" s="12"/>
+      <c r="P12" s="12"/>
+      <c r="Q12" s="12"/>
+      <c r="R12" s="12"/>
+      <c r="S12" s="12"/>
+      <c r="T12" s="12"/>
+      <c r="U12" s="12"/>
+      <c r="V12" s="12"/>
+      <c r="W12" s="12"/>
+      <c r="X12" s="12"/>
+      <c r="Y12" s="12"/>
+      <c r="Z12" s="12"/>
+      <c r="AA12" s="12"/>
+      <c r="AB12" s="12"/>
     </row>
     <row r="14" spans="2:28" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="13"/>
-      <c r="K14" s="13"/>
-      <c r="L14" s="13"/>
-      <c r="M14" s="13"/>
-      <c r="N14" s="13"/>
-      <c r="O14" s="13"/>
-      <c r="P14" s="13"/>
-      <c r="Q14" s="13"/>
-      <c r="R14" s="13"/>
-      <c r="S14" s="13"/>
-      <c r="T14" s="13"/>
-      <c r="U14" s="13"/>
-      <c r="V14" s="13"/>
-      <c r="W14" s="13"/>
-      <c r="X14" s="13"/>
-      <c r="Y14" s="13"/>
-      <c r="Z14" s="13"/>
-      <c r="AA14" s="13"/>
-      <c r="AB14" s="13"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="12"/>
+      <c r="M14" s="12"/>
+      <c r="N14" s="12"/>
+      <c r="O14" s="12"/>
+      <c r="P14" s="12"/>
+      <c r="Q14" s="12"/>
+      <c r="R14" s="12"/>
+      <c r="S14" s="12"/>
+      <c r="T14" s="12"/>
+      <c r="U14" s="12"/>
+      <c r="V14" s="12"/>
+      <c r="W14" s="12"/>
+      <c r="X14" s="12"/>
+      <c r="Y14" s="12"/>
+      <c r="Z14" s="12"/>
+      <c r="AA14" s="12"/>
+      <c r="AB14" s="12"/>
     </row>
     <row r="16" spans="2:28" ht="21.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="13" t="s">
+      <c r="B16" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="13"/>
-      <c r="K16" s="13"/>
-      <c r="L16" s="13"/>
-      <c r="M16" s="13"/>
-      <c r="N16" s="13"/>
-      <c r="O16" s="13"/>
-      <c r="P16" s="13"/>
-      <c r="Q16" s="13"/>
-      <c r="R16" s="13"/>
-      <c r="S16" s="13"/>
-      <c r="T16" s="13"/>
-      <c r="U16" s="13"/>
-      <c r="V16" s="13"/>
-      <c r="W16" s="13"/>
-      <c r="X16" s="13"/>
-      <c r="Y16" s="13"/>
-      <c r="Z16" s="13"/>
-      <c r="AA16" s="13"/>
-      <c r="AB16" s="13"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="12"/>
+      <c r="N16" s="12"/>
+      <c r="O16" s="12"/>
+      <c r="P16" s="12"/>
+      <c r="Q16" s="12"/>
+      <c r="R16" s="12"/>
+      <c r="S16" s="12"/>
+      <c r="T16" s="12"/>
+      <c r="U16" s="12"/>
+      <c r="V16" s="12"/>
+      <c r="W16" s="12"/>
+      <c r="X16" s="12"/>
+      <c r="Y16" s="12"/>
+      <c r="Z16" s="12"/>
+      <c r="AA16" s="12"/>
+      <c r="AB16" s="12"/>
     </row>
     <row r="18" spans="2:28" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="13" t="s">
+      <c r="B18" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="13"/>
-      <c r="K18" s="13"/>
-      <c r="L18" s="13"/>
-      <c r="M18" s="13"/>
-      <c r="N18" s="13"/>
-      <c r="O18" s="13"/>
-      <c r="P18" s="13"/>
-      <c r="Q18" s="13"/>
-      <c r="R18" s="13"/>
-      <c r="S18" s="13"/>
-      <c r="T18" s="13"/>
-      <c r="U18" s="13"/>
-      <c r="V18" s="13"/>
-      <c r="W18" s="13"/>
-      <c r="X18" s="13"/>
-      <c r="Y18" s="13"/>
-      <c r="Z18" s="13"/>
-      <c r="AA18" s="13"/>
-      <c r="AB18" s="13"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="12"/>
+      <c r="K18" s="12"/>
+      <c r="L18" s="12"/>
+      <c r="M18" s="12"/>
+      <c r="N18" s="12"/>
+      <c r="O18" s="12"/>
+      <c r="P18" s="12"/>
+      <c r="Q18" s="12"/>
+      <c r="R18" s="12"/>
+      <c r="S18" s="12"/>
+      <c r="T18" s="12"/>
+      <c r="U18" s="12"/>
+      <c r="V18" s="12"/>
+      <c r="W18" s="12"/>
+      <c r="X18" s="12"/>
+      <c r="Y18" s="12"/>
+      <c r="Z18" s="12"/>
+      <c r="AA18" s="12"/>
+      <c r="AB18" s="12"/>
     </row>
     <row r="19" spans="2:28" ht="35.1" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="20" spans="2:28" x14ac:dyDescent="0.2">
-      <c r="B20" s="12" t="s">
+      <c r="B20" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="12"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
       <c r="I20" s="1"/>
     </row>
     <row r="21" spans="2:28" x14ac:dyDescent="0.2">
@@ -1202,331 +1236,366 @@
       <c r="AB22" s="4"/>
     </row>
     <row r="23" spans="2:28" x14ac:dyDescent="0.2">
-      <c r="B23" s="11" t="s">
+      <c r="B23" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="11"/>
-      <c r="I23" s="5"/>
-      <c r="J23" s="5"/>
-      <c r="K23" s="5"/>
-      <c r="L23" s="5"/>
-      <c r="M23" s="5"/>
-      <c r="N23" s="5"/>
-      <c r="O23" s="5"/>
-      <c r="P23" s="5"/>
-      <c r="Q23" s="5"/>
-      <c r="R23" s="5"/>
-      <c r="S23" s="5"/>
-      <c r="T23" s="5"/>
-      <c r="U23" s="5"/>
-      <c r="V23" s="5"/>
-      <c r="W23" s="5"/>
-      <c r="X23" s="5"/>
-      <c r="Y23" s="5"/>
-      <c r="Z23" s="5"/>
-      <c r="AA23" s="5"/>
-      <c r="AB23" s="5"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="19"/>
+      <c r="I23" s="14"/>
+      <c r="J23" s="16"/>
+      <c r="K23" s="16"/>
+      <c r="L23" s="16"/>
+      <c r="M23" s="16"/>
+      <c r="N23" s="16"/>
+      <c r="O23" s="16"/>
+      <c r="P23" s="16"/>
+      <c r="Q23" s="16"/>
+      <c r="R23" s="16"/>
+      <c r="S23" s="16"/>
+      <c r="T23" s="16"/>
+      <c r="U23" s="16"/>
+      <c r="V23" s="16"/>
+      <c r="W23" s="16"/>
+      <c r="X23" s="16"/>
+      <c r="Y23" s="16"/>
+      <c r="Z23" s="14"/>
+      <c r="AA23" s="16"/>
+      <c r="AB23" s="14"/>
     </row>
     <row r="24" spans="2:28" x14ac:dyDescent="0.2">
-      <c r="I24" s="4"/>
-      <c r="J24" s="4"/>
-      <c r="K24" s="4"/>
-      <c r="L24" s="4"/>
-      <c r="M24" s="4"/>
-      <c r="N24" s="4"/>
-      <c r="O24" s="4"/>
-      <c r="P24" s="4"/>
-      <c r="Q24" s="4"/>
-      <c r="R24" s="4"/>
-      <c r="S24" s="4"/>
-      <c r="T24" s="4"/>
-      <c r="U24" s="4"/>
-      <c r="V24" s="4"/>
-      <c r="W24" s="4"/>
-      <c r="X24" s="4"/>
-      <c r="Y24" s="4"/>
-      <c r="Z24" s="4"/>
-      <c r="AA24" s="4"/>
-      <c r="AB24" s="4"/>
+      <c r="B24" s="20"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="21"/>
+      <c r="I24" s="15"/>
+      <c r="J24" s="17"/>
+      <c r="K24" s="17"/>
+      <c r="L24" s="17"/>
+      <c r="M24" s="17"/>
+      <c r="N24" s="17"/>
+      <c r="O24" s="17"/>
+      <c r="P24" s="17"/>
+      <c r="Q24" s="17"/>
+      <c r="R24" s="17"/>
+      <c r="S24" s="17"/>
+      <c r="T24" s="17"/>
+      <c r="U24" s="17"/>
+      <c r="V24" s="17"/>
+      <c r="W24" s="17"/>
+      <c r="X24" s="17"/>
+      <c r="Y24" s="17"/>
+      <c r="Z24" s="15"/>
+      <c r="AA24" s="17"/>
+      <c r="AB24" s="15"/>
     </row>
     <row r="25" spans="2:28" x14ac:dyDescent="0.2">
-      <c r="B25" s="11" t="s">
+      <c r="B25" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C25" s="11"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="11"/>
-      <c r="I25" s="5"/>
-      <c r="J25" s="5"/>
-      <c r="K25" s="5"/>
-      <c r="L25" s="5"/>
-      <c r="M25" s="5"/>
-      <c r="N25" s="5"/>
-      <c r="O25" s="5"/>
-      <c r="P25" s="5"/>
-      <c r="Q25" s="5"/>
-      <c r="R25" s="5"/>
-      <c r="S25" s="5"/>
-      <c r="T25" s="5"/>
-      <c r="U25" s="5"/>
-      <c r="V25" s="5"/>
-      <c r="W25" s="5"/>
-      <c r="X25" s="5"/>
-      <c r="Y25" s="5"/>
-      <c r="Z25" s="5"/>
-      <c r="AA25" s="5"/>
-      <c r="AB25" s="5"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="19"/>
+      <c r="I25" s="14"/>
+      <c r="J25" s="16"/>
+      <c r="K25" s="16"/>
+      <c r="L25" s="16"/>
+      <c r="M25" s="16"/>
+      <c r="N25" s="16"/>
+      <c r="O25" s="16"/>
+      <c r="P25" s="16"/>
+      <c r="Q25" s="16"/>
+      <c r="R25" s="16"/>
+      <c r="S25" s="16"/>
+      <c r="T25" s="16"/>
+      <c r="U25" s="16"/>
+      <c r="V25" s="16"/>
+      <c r="W25" s="16"/>
+      <c r="X25" s="16"/>
+      <c r="Y25" s="16"/>
+      <c r="Z25" s="14"/>
+      <c r="AA25" s="16"/>
+      <c r="AB25" s="14"/>
     </row>
     <row r="26" spans="2:28" x14ac:dyDescent="0.2">
-      <c r="I26" s="4"/>
-      <c r="J26" s="4"/>
-      <c r="K26" s="4"/>
-      <c r="L26" s="4"/>
-      <c r="M26" s="4"/>
-      <c r="N26" s="4"/>
-      <c r="O26" s="4"/>
-      <c r="P26" s="4"/>
-      <c r="Q26" s="4"/>
-      <c r="R26" s="4"/>
-      <c r="S26" s="4"/>
-      <c r="T26" s="4"/>
-      <c r="U26" s="4"/>
-      <c r="V26" s="4"/>
-      <c r="W26" s="4"/>
-      <c r="X26" s="4"/>
-      <c r="Y26" s="4"/>
-      <c r="Z26" s="4"/>
-      <c r="AA26" s="4"/>
-      <c r="AB26" s="4"/>
+      <c r="B26" s="20"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="21"/>
+      <c r="I26" s="15"/>
+      <c r="J26" s="17"/>
+      <c r="K26" s="17"/>
+      <c r="L26" s="17"/>
+      <c r="M26" s="17"/>
+      <c r="N26" s="17"/>
+      <c r="O26" s="17"/>
+      <c r="P26" s="17"/>
+      <c r="Q26" s="17"/>
+      <c r="R26" s="17"/>
+      <c r="S26" s="17"/>
+      <c r="T26" s="17"/>
+      <c r="U26" s="17"/>
+      <c r="V26" s="17"/>
+      <c r="W26" s="17"/>
+      <c r="X26" s="17"/>
+      <c r="Y26" s="17"/>
+      <c r="Z26" s="15"/>
+      <c r="AA26" s="17"/>
+      <c r="AB26" s="15"/>
     </row>
     <row r="27" spans="2:28" x14ac:dyDescent="0.2">
-      <c r="B27" s="11" t="s">
+      <c r="B27" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C27" s="11"/>
-      <c r="D27" s="11"/>
-      <c r="E27" s="11"/>
-      <c r="F27" s="11"/>
-      <c r="G27" s="11"/>
-      <c r="H27" s="11"/>
-      <c r="I27" s="5"/>
-      <c r="J27" s="5"/>
-      <c r="K27" s="5"/>
-      <c r="L27" s="5"/>
-      <c r="M27" s="5"/>
-      <c r="N27" s="5"/>
-      <c r="O27" s="5"/>
-      <c r="P27" s="5"/>
-      <c r="Q27" s="5"/>
-      <c r="R27" s="5"/>
-      <c r="S27" s="5"/>
-      <c r="T27" s="5"/>
-      <c r="U27" s="5"/>
-      <c r="V27" s="5"/>
-      <c r="W27" s="5"/>
-      <c r="X27" s="5"/>
-      <c r="Y27" s="5"/>
-      <c r="Z27" s="5"/>
-      <c r="AA27" s="5"/>
-      <c r="AB27" s="5"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="19"/>
+      <c r="I27" s="14"/>
+      <c r="J27" s="16"/>
+      <c r="K27" s="16"/>
+      <c r="L27" s="16"/>
+      <c r="M27" s="16"/>
+      <c r="N27" s="16"/>
+      <c r="O27" s="16"/>
+      <c r="P27" s="16"/>
+      <c r="Q27" s="16"/>
+      <c r="R27" s="16"/>
+      <c r="S27" s="16"/>
+      <c r="T27" s="16"/>
+      <c r="U27" s="16"/>
+      <c r="V27" s="16"/>
+      <c r="W27" s="16"/>
+      <c r="X27" s="16"/>
+      <c r="Y27" s="16"/>
+      <c r="Z27" s="14"/>
+      <c r="AA27" s="16"/>
+      <c r="AB27" s="14"/>
     </row>
     <row r="28" spans="2:28" x14ac:dyDescent="0.2">
-      <c r="I28" s="4"/>
-      <c r="J28" s="4"/>
-      <c r="K28" s="4"/>
-      <c r="L28" s="4"/>
-      <c r="M28" s="4"/>
-      <c r="N28" s="4"/>
-      <c r="O28" s="4"/>
-      <c r="P28" s="4"/>
-      <c r="Q28" s="4"/>
-      <c r="R28" s="4"/>
-      <c r="S28" s="4"/>
-      <c r="T28" s="4"/>
-      <c r="U28" s="4"/>
-      <c r="V28" s="4"/>
-      <c r="W28" s="4"/>
-      <c r="X28" s="4"/>
-      <c r="Y28" s="4"/>
-      <c r="Z28" s="4"/>
-      <c r="AA28" s="4"/>
-      <c r="AB28" s="4"/>
+      <c r="B28" s="20"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="20"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="20"/>
+      <c r="H28" s="21"/>
+      <c r="I28" s="15"/>
+      <c r="J28" s="17"/>
+      <c r="K28" s="17"/>
+      <c r="L28" s="17"/>
+      <c r="M28" s="17"/>
+      <c r="N28" s="17"/>
+      <c r="O28" s="17"/>
+      <c r="P28" s="17"/>
+      <c r="Q28" s="17"/>
+      <c r="R28" s="17"/>
+      <c r="S28" s="17"/>
+      <c r="T28" s="17"/>
+      <c r="U28" s="17"/>
+      <c r="V28" s="17"/>
+      <c r="W28" s="17"/>
+      <c r="X28" s="17"/>
+      <c r="Y28" s="17"/>
+      <c r="Z28" s="15"/>
+      <c r="AA28" s="17"/>
+      <c r="AB28" s="15"/>
     </row>
     <row r="29" spans="2:28" x14ac:dyDescent="0.2">
-      <c r="B29" s="11" t="s">
+      <c r="B29" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="C29" s="11"/>
-      <c r="D29" s="11"/>
-      <c r="E29" s="11"/>
-      <c r="F29" s="11"/>
-      <c r="G29" s="11"/>
-      <c r="H29" s="11"/>
-      <c r="I29" s="5"/>
-      <c r="J29" s="5"/>
-      <c r="K29" s="5"/>
-      <c r="L29" s="5"/>
-      <c r="M29" s="5"/>
-      <c r="N29" s="5"/>
-      <c r="O29" s="5"/>
-      <c r="P29" s="5"/>
-      <c r="Q29" s="5"/>
-      <c r="R29" s="5"/>
-      <c r="S29" s="5"/>
-      <c r="T29" s="5"/>
-      <c r="U29" s="5"/>
-      <c r="V29" s="5"/>
-      <c r="W29" s="5"/>
-      <c r="X29" s="5"/>
-      <c r="Y29" s="5"/>
-      <c r="Z29" s="5"/>
-      <c r="AA29" s="5"/>
-      <c r="AB29" s="5"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
+      <c r="H29" s="19"/>
+      <c r="I29" s="14"/>
+      <c r="J29" s="16"/>
+      <c r="K29" s="16"/>
+      <c r="L29" s="16"/>
+      <c r="M29" s="16"/>
+      <c r="N29" s="16"/>
+      <c r="O29" s="16"/>
+      <c r="P29" s="16"/>
+      <c r="Q29" s="16"/>
+      <c r="R29" s="16"/>
+      <c r="S29" s="16"/>
+      <c r="T29" s="16"/>
+      <c r="U29" s="16"/>
+      <c r="V29" s="16"/>
+      <c r="W29" s="16"/>
+      <c r="X29" s="16"/>
+      <c r="Y29" s="16"/>
+      <c r="Z29" s="14"/>
+      <c r="AA29" s="16"/>
+      <c r="AB29" s="14"/>
     </row>
     <row r="30" spans="2:28" x14ac:dyDescent="0.2">
-      <c r="I30" s="4"/>
-      <c r="J30" s="4"/>
-      <c r="K30" s="4"/>
-      <c r="L30" s="4"/>
-      <c r="M30" s="4"/>
-      <c r="N30" s="4"/>
-      <c r="O30" s="4"/>
-      <c r="P30" s="4"/>
-      <c r="Q30" s="4"/>
-      <c r="R30" s="4"/>
-      <c r="S30" s="4"/>
-      <c r="T30" s="4"/>
-      <c r="U30" s="4"/>
-      <c r="V30" s="4"/>
-      <c r="W30" s="4"/>
-      <c r="X30" s="4"/>
-      <c r="Y30" s="4"/>
-      <c r="Z30" s="4"/>
-      <c r="AA30" s="4"/>
-      <c r="AB30" s="4"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="21"/>
+      <c r="I30" s="15"/>
+      <c r="J30" s="17"/>
+      <c r="K30" s="17"/>
+      <c r="L30" s="17"/>
+      <c r="M30" s="17"/>
+      <c r="N30" s="17"/>
+      <c r="O30" s="17"/>
+      <c r="P30" s="17"/>
+      <c r="Q30" s="17"/>
+      <c r="R30" s="17"/>
+      <c r="S30" s="17"/>
+      <c r="T30" s="17"/>
+      <c r="U30" s="17"/>
+      <c r="V30" s="17"/>
+      <c r="W30" s="17"/>
+      <c r="X30" s="17"/>
+      <c r="Y30" s="17"/>
+      <c r="Z30" s="15"/>
+      <c r="AA30" s="17"/>
+      <c r="AB30" s="15"/>
     </row>
     <row r="31" spans="2:28" x14ac:dyDescent="0.2">
-      <c r="B31" s="11" t="s">
+      <c r="B31" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C31" s="11"/>
-      <c r="D31" s="11"/>
-      <c r="E31" s="11"/>
-      <c r="F31" s="11"/>
-      <c r="G31" s="11"/>
-      <c r="H31" s="11"/>
-      <c r="I31" s="5"/>
-      <c r="J31" s="5"/>
-      <c r="K31" s="5"/>
-      <c r="L31" s="5"/>
-      <c r="M31" s="5"/>
-      <c r="N31" s="5"/>
-      <c r="O31" s="5"/>
-      <c r="P31" s="5"/>
-      <c r="Q31" s="5"/>
-      <c r="R31" s="5"/>
-      <c r="S31" s="5"/>
-      <c r="T31" s="5"/>
-      <c r="U31" s="5"/>
-      <c r="V31" s="5"/>
-      <c r="W31" s="5"/>
-      <c r="X31" s="5"/>
-      <c r="Y31" s="5"/>
-      <c r="Z31" s="5"/>
-      <c r="AA31" s="5"/>
-      <c r="AB31" s="5"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
+      <c r="H31" s="19"/>
+      <c r="I31" s="14"/>
+      <c r="J31" s="16"/>
+      <c r="K31" s="16"/>
+      <c r="L31" s="16"/>
+      <c r="M31" s="16"/>
+      <c r="N31" s="16"/>
+      <c r="O31" s="16"/>
+      <c r="P31" s="16"/>
+      <c r="Q31" s="16"/>
+      <c r="R31" s="16"/>
+      <c r="S31" s="16"/>
+      <c r="T31" s="16"/>
+      <c r="U31" s="16"/>
+      <c r="V31" s="16"/>
+      <c r="W31" s="16"/>
+      <c r="X31" s="16"/>
+      <c r="Y31" s="16"/>
+      <c r="Z31" s="14"/>
+      <c r="AA31" s="16"/>
+      <c r="AB31" s="14"/>
     </row>
     <row r="32" spans="2:28" x14ac:dyDescent="0.2">
-      <c r="I32" s="4"/>
-      <c r="J32" s="4"/>
-      <c r="K32" s="4"/>
-      <c r="L32" s="4"/>
-      <c r="M32" s="4"/>
-      <c r="N32" s="4"/>
-      <c r="O32" s="4"/>
-      <c r="P32" s="4"/>
-      <c r="Q32" s="4"/>
-      <c r="R32" s="4"/>
-      <c r="S32" s="4"/>
-      <c r="T32" s="4"/>
-      <c r="U32" s="4"/>
-      <c r="V32" s="4"/>
-      <c r="W32" s="4"/>
-      <c r="X32" s="4"/>
-      <c r="Y32" s="4"/>
-      <c r="Z32" s="4"/>
-      <c r="AA32" s="4"/>
-      <c r="AB32" s="4"/>
+      <c r="B32" s="20"/>
+      <c r="C32" s="20"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="20"/>
+      <c r="H32" s="21"/>
+      <c r="I32" s="15"/>
+      <c r="J32" s="17"/>
+      <c r="K32" s="17"/>
+      <c r="L32" s="17"/>
+      <c r="M32" s="17"/>
+      <c r="N32" s="17"/>
+      <c r="O32" s="17"/>
+      <c r="P32" s="17"/>
+      <c r="Q32" s="17"/>
+      <c r="R32" s="17"/>
+      <c r="S32" s="17"/>
+      <c r="T32" s="17"/>
+      <c r="U32" s="17"/>
+      <c r="V32" s="17"/>
+      <c r="W32" s="17"/>
+      <c r="X32" s="17"/>
+      <c r="Y32" s="17"/>
+      <c r="Z32" s="15"/>
+      <c r="AA32" s="17"/>
+      <c r="AB32" s="15"/>
     </row>
     <row r="33" spans="2:28" x14ac:dyDescent="0.2">
-      <c r="B33" s="11" t="s">
+      <c r="B33" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="C33" s="11"/>
-      <c r="D33" s="11"/>
-      <c r="E33" s="11"/>
-      <c r="F33" s="11"/>
-      <c r="G33" s="11"/>
-      <c r="H33" s="11"/>
-      <c r="I33" s="5"/>
-      <c r="J33" s="5"/>
-      <c r="K33" s="5"/>
-      <c r="L33" s="5"/>
-      <c r="M33" s="5"/>
-      <c r="N33" s="5"/>
-      <c r="O33" s="5"/>
-      <c r="P33" s="5"/>
-      <c r="Q33" s="5"/>
-      <c r="R33" s="5"/>
-      <c r="S33" s="5"/>
-      <c r="T33" s="5"/>
-      <c r="U33" s="5"/>
-      <c r="V33" s="5"/>
-      <c r="W33" s="5"/>
-      <c r="X33" s="5"/>
-      <c r="Y33" s="5"/>
-      <c r="Z33" s="5"/>
-      <c r="AA33" s="5"/>
-      <c r="AB33" s="5"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
+      <c r="H33" s="19"/>
+      <c r="I33" s="14"/>
+      <c r="J33" s="16"/>
+      <c r="K33" s="16"/>
+      <c r="L33" s="16"/>
+      <c r="M33" s="16"/>
+      <c r="N33" s="16"/>
+      <c r="O33" s="16"/>
+      <c r="P33" s="16"/>
+      <c r="Q33" s="16"/>
+      <c r="R33" s="16"/>
+      <c r="S33" s="16"/>
+      <c r="T33" s="16"/>
+      <c r="U33" s="16"/>
+      <c r="V33" s="16"/>
+      <c r="W33" s="16"/>
+      <c r="X33" s="16"/>
+      <c r="Y33" s="16"/>
+      <c r="Z33" s="14"/>
+      <c r="AA33" s="16"/>
+      <c r="AB33" s="14"/>
     </row>
     <row r="36" spans="2:28" x14ac:dyDescent="0.2">
-      <c r="B36" s="12" t="s">
+      <c r="B36" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C36" s="12"/>
-      <c r="D36" s="12"/>
-      <c r="E36" s="12"/>
-      <c r="F36" s="12"/>
-      <c r="G36" s="12"/>
-      <c r="H36" s="12"/>
-      <c r="I36" s="12"/>
-      <c r="J36" s="12"/>
-      <c r="K36" s="12"/>
-      <c r="L36" s="12"/>
-      <c r="M36" s="12"/>
-      <c r="N36" s="12"/>
-      <c r="O36" s="12"/>
-      <c r="P36" s="12"/>
-      <c r="Q36" s="12"/>
-      <c r="R36" s="12"/>
-      <c r="S36" s="12"/>
-      <c r="T36" s="12"/>
-      <c r="U36" s="12"/>
-      <c r="V36" s="12"/>
-      <c r="W36" s="12"/>
-      <c r="X36" s="12"/>
-      <c r="Y36" s="12"/>
-      <c r="Z36" s="12"/>
-      <c r="AA36" s="12"/>
-      <c r="AB36" s="12"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
+      <c r="H36" s="13"/>
+      <c r="I36" s="13"/>
+      <c r="J36" s="13"/>
+      <c r="K36" s="13"/>
+      <c r="L36" s="13"/>
+      <c r="M36" s="13"/>
+      <c r="N36" s="13"/>
+      <c r="O36" s="13"/>
+      <c r="P36" s="13"/>
+      <c r="Q36" s="13"/>
+      <c r="R36" s="13"/>
+      <c r="S36" s="13"/>
+      <c r="T36" s="13"/>
+      <c r="U36" s="13"/>
+      <c r="V36" s="13"/>
+      <c r="W36" s="13"/>
+      <c r="X36" s="13"/>
+      <c r="Y36" s="13"/>
+      <c r="Z36" s="13"/>
+      <c r="AA36" s="13"/>
+      <c r="AB36" s="13"/>
     </row>
     <row r="38" spans="2:28" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="39" spans="2:28" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1802,11 +1871,6 @@
     </customSheetView>
   </customSheetViews>
   <mergeCells count="16">
-    <mergeCell ref="B4:AB4"/>
-    <mergeCell ref="B6:AB6"/>
-    <mergeCell ref="B8:AB8"/>
-    <mergeCell ref="B10:AB10"/>
-    <mergeCell ref="B18:AB18"/>
     <mergeCell ref="B31:H31"/>
     <mergeCell ref="B33:H33"/>
     <mergeCell ref="B36:AB36"/>
@@ -1818,6 +1882,11 @@
     <mergeCell ref="B23:H23"/>
     <mergeCell ref="B25:H25"/>
     <mergeCell ref="B27:H27"/>
+    <mergeCell ref="B4:AB4"/>
+    <mergeCell ref="B6:AB6"/>
+    <mergeCell ref="B8:AB8"/>
+    <mergeCell ref="B10:AB10"/>
+    <mergeCell ref="B18:AB18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>